<commit_message>
add final version of results
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\O-SE-R\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA11485-9A3C-479C-9112-30D123CDEAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2655BE57-0CB7-4FDC-8BFA-BC239EDCB543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D53EE773-7489-46E7-84B2-C460A77A286B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="80">
   <si>
     <t>Actual Number of Classes</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>AGGREGATE RESULTS</t>
+  </si>
+  <si>
+    <t>Actual Number of Associations</t>
   </si>
 </sst>
 </file>
@@ -320,10 +323,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE34251-BC23-4ED1-BFB5-428C3A8634CA}">
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" topLeftCell="B61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2502,12 +2506,33 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
+      <c r="A77" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" t="s">
+        <v>79</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78">
@@ -2519,7 +2544,7 @@
         <v>274</v>
       </c>
       <c r="C78">
-        <f t="shared" ref="C78:H78" si="0">SUM(C3:C72)</f>
+        <f t="shared" ref="C78:H79" si="0">SUM(C3:C72)</f>
         <v>144</v>
       </c>
       <c r="D78">

</xml_diff>